<commit_message>
Buy and sell scoring
</commit_message>
<xml_diff>
--- a/portfolio_history_detailed.xlsx
+++ b/portfolio_history_detailed.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +520,1206 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>45603.41805730324</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.01844300</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>74952.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1382.34</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Death Cross detected - Short MA (70774.524) crossed below Long MA (74068.20583333333) with RSI (52.55089048487729).</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1382.34</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.18443000</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1382.34</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1382.34</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>45603.41820510416</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.01844300</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>74965.46</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1382.59</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Death Cross detected - Short MA (70775.651) crossed below Long MA (74068.39366666667) with RSI (52.566090388861255).</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1382.59</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.18443000</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1382.59</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2764.93</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>4.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>45603.41835085648</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.01844300</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>74981.25</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1382.88</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Death Cross detected - Short MA (70777.393) crossed below Long MA (74068.684) with RSI (52.58960213504466).</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1382.88</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.18443000</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>1382.88</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4147.81</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>6.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>45603.41849825231</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.01844300</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>74993.23</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1383.10</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Death Cross detected - Short MA (70778.113) crossed below Long MA (74068.804) with RSI (52.59932610779406).</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1383.10</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.18443000</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>1383.10</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>5530.91</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>8.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>45603.41864084491</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.01844300</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>74993.55</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1383.11</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Death Cross detected - Short MA (70778.89499999999) crossed below Long MA (74068.93433333334) with RSI (52.60989149725558).</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1383.11</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.18443000</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>1383.11</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>6914.01</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>68720.13</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>10.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>45603.54926792183</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>75984.02</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>280.46</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>280.46</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>280.46</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>280.46</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>45603.5494055668</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>75964.77</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>560.84</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>45603.54954002484</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>75963.99</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>841.23</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>45603.54967468484</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>75962.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>1121.60</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>45603.54981223203</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>75964.23</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>1401.99</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>1.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>45603.54994388673</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>75964.77</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>280.39</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>1682.37</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>45603.55008576949</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>75964.01</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1962.75</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>45603.55022342513</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>75964.01</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>280.38</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2243.14</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>45603.55036683186</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>75900.00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>280.15</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>280.15</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>280.15</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2523.28</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>45603.55049978279</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.00369100</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>75895.23</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>280.13</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Take-profit triggered at 0.0.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>280.13</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.03691000</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>280.13</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2803.41</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>79822.13</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>3.51</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bugs small portifolio
</commit_message>
<xml_diff>
--- a/portfolio_history_detailed.xlsx
+++ b/portfolio_history_detailed.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S167"/>
+  <dimension ref="A1:S170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15927,7 +15927,7 @@
     </row>
     <row r="164">
       <c r="A164" s="3" t="n">
-        <v>45604.85270664041</v>
+        <v>45604.85270664352</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -16022,7 +16022,7 @@
     </row>
     <row r="165">
       <c r="A165" s="3" t="n">
-        <v>45604.85286658546</v>
+        <v>45604.85286658565</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -16117,7 +16117,7 @@
     </row>
     <row r="166">
       <c r="A166" s="3" t="n">
-        <v>45604.85302367982</v>
+        <v>45604.85302368055</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -16212,7 +16212,7 @@
     </row>
     <row r="167">
       <c r="A167" s="3" t="n">
-        <v>45604.85318097223</v>
+        <v>45604.85318097222</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -16302,6 +16302,291 @@
       <c r="S167" t="inlineStr">
         <is>
           <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="3" t="n">
+        <v>45606.58139018519</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>0.01707000</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>79699.33</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>1360.47</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>1360.47</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>69581.86</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>0.17070000</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>1360.47</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>1360.47</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>69581.86</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P168" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R168" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>Profit of 1360.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="3" t="n">
+        <v>45606.58153751157</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0.01707000</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>79697.13</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>1360.43</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>1360.43</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>69581.86</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>0.17070000</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>1360.43</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>2720.90</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>69581.86</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P169" t="inlineStr">
+        <is>
+          <t>3.91</t>
+        </is>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R169" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S169" t="inlineStr">
+        <is>
+          <t>Profit of 1360.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="3" t="n">
+        <v>45606.58189127497</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0.01365800</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>79689.02</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>1088.39</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>1088.39</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>72301.14</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>0.13658000</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>1088.39</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>1088.39</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>72301.14</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P170" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R170" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>Profit of 1088.39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new condicion small - consecultives bloks
</commit_message>
<xml_diff>
--- a/portfolio_history_detailed.xlsx
+++ b/portfolio_history_detailed.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S170"/>
+  <dimension ref="A1:S178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16497,7 +16497,7 @@
     </row>
     <row r="170">
       <c r="A170" s="3" t="n">
-        <v>45606.58189127497</v>
+        <v>45606.58189127315</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -16587,6 +16587,766 @@
       <c r="S170" t="inlineStr">
         <is>
           <t>Profit of 1088.39</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="3" t="n">
+        <v>45607.64172494213</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>0.01229300</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>84415.88</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>1037.72</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>73388.77</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>0.12293000</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>1037.72</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>72351.05</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R171" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="3" t="n">
+        <v>45607.64188423611</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>0.01229300</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>84467.24</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>0.12293000</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P172" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R172" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S172" t="inlineStr">
+        <is>
+          <t>Profit of 1038.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="3" t="n">
+        <v>45607.64204055555</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>0.01229300</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>84467.24</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>0.12293000</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>2076.71</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P173" t="inlineStr">
+        <is>
+          <t>2.83</t>
+        </is>
+      </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R173" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
+          <t>Profit of 1038.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="3" t="n">
+        <v>45607.64218829861</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>0.01229300</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>84467.24</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>0.12293000</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>1038.36</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>3115.07</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>73389.40</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P174" t="inlineStr">
+        <is>
+          <t>4.24</t>
+        </is>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R174" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S174" t="inlineStr">
+        <is>
+          <t>Profit of 1038.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="3" t="n">
+        <v>45607.66492768518</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0.00983500</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>85537.14</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>841.26</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>841.26</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>75071.24</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>0.09835000</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>841.26</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>841.26</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>75071.24</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P175" t="inlineStr">
+        <is>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R175" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S175" t="inlineStr">
+        <is>
+          <t>Profit of 841.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="3" t="n">
+        <v>45607.66507328704</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0.00983500</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>85536.70</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>841.25</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>841.25</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>75071.24</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>0.09835000</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>841.25</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>1682.51</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>75071.24</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P176" t="inlineStr">
+        <is>
+          <t>2.24</t>
+        </is>
+      </c>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R176" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S176" t="inlineStr">
+        <is>
+          <t>Profit of 841.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="3" t="n">
+        <v>45607.72814283278</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>0.00472500</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>86849.99</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>79455.73</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>0.04725000</t>
+        </is>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>79045.36</t>
+        </is>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R177" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S177" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="3" t="n">
+        <v>45607.7282989224</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>0.00472500</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>86849.99</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>79455.73</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>0.04725000</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>410.37</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>79455.73</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P178" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R178" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
+          <t>Profit of 410.37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testando nova estrategia trade fast
</commit_message>
<xml_diff>
--- a/portfolio_history_detailed.xlsx
+++ b/portfolio_history_detailed.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,8 +536,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45609.69485166704</v>
+      <c r="A2" s="3" t="n">
+        <v>45609.69485166667</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -630,8 +631,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45609.69515758493</v>
+      <c r="A3" s="3" t="n">
+        <v>45609.69515758102</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -725,8 +726,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45609.69532276132</v>
+      <c r="A4" s="3" t="n">
+        <v>45609.6953227662</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -820,8 +821,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45609.69547674359</v>
+      <c r="A5" s="3" t="n">
+        <v>45609.69547674769</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -915,8 +916,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45609.69562459309</v>
+      <c r="A6" s="3" t="n">
+        <v>45609.6956245949</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1004,6 +1005,2096 @@
         </is>
       </c>
       <c r="S6" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>45614.48819452546</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>90586.57</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Profit of 9.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>45614.48835487269</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>90402.98</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>9.04</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>9.04</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>80664.13</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>45614.48851163194</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>90648.31</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>80655.07</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>45614.48866827547</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>90668.80</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>80646.00</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>45614.48883115741</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>90684.98</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>45614.488981875</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>90704.80</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>80673.17</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>80627.86</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>45614.48913292824</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>90704.80</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>18.13</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Profit of 9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>45614.48928086805</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>90719.19</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>27.20</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Profit of 9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>45614.48942886574</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>90739.21</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>36.27</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Profit of 9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>45614.48958572916</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>90740.30</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>45.35</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Profit of 9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>45614.48986085648</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>90740.30</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>54.42</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>80636.93</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Profit of 9.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>45614.49016655092</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>90672.30</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>80682.00</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>80672.94</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>45614.49032334491</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>90654.93</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>80682.00</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>80663.87</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>45614.49047407407</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>90622.30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>80682.00</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>80654.81</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>45614.49062893519</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>90600.20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>80682.00</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>80645.75</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>45614.49077663194</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>90588.33</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>80682.00</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>9.06</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>80636.69</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Loss of 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>45614.54689128472</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>92572.21</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Profit of 9.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>45614.54704665509</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>92181.82</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>9.22</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>9.22</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>9.22</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>18.48</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Profit of 9.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>45614.54720480324</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>92572.21</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>27.73</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Profit of 9.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>45614.54737438657</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>92572.21</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0.00047000</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>9.26</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>36.99</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>80645.95</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Profit of 9.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>45614.54932795719</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>92465.42</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Venda para lucro a curto prazo em carteira pequena com limite de vendas consecutivas</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>80673.56</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>80673.56</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Profit of 9.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>45614.54978762715</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.00010000</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>92004.53</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>9.20</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Compra em oportunidade de curto prazo com base em indicadores e limite de compras consecutivas</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>80673.56</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.00057000</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>9.20</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>80664.36</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
         <is>
           <t>Loss of 0.00</t>
         </is>

</xml_diff>